<commit_message>
fix gitignore and dataset
</commit_message>
<xml_diff>
--- a/data/processed/7.xlsx
+++ b/data/processed/7.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraphRAG\result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NeoGRAG\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF531C44-7B70-4D94-9AF8-9130796F9483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BCEBD0-2ACE-4EF6-9C90-99020CC84C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,9 +91,6 @@
     <t xml:space="preserve">chương III  ĐÁNH GIÁ KẾT QUẢ HỌC TẬP  điều 21. đánh giá học phần 1. học phần lý thuyết hoặc học phần lý thuyết kết hợp thực hành điểm học phần được đánh giá qua tối thiểu hai điểm thành phần như điểm bài tập, điểm kiểm tra giữa kỳ, điểm thực hành, điểm đánh giá nhận thức, điểm tham gia thảo luận, điểm chuyên cần, điểm đồ án,... và điểm thi kết thúc học phần. thi kết thúc học phần là bắt buộc. phương pháp đánh giá học phần được công bố trong đề cương chi tiết học phần. tổ chức kỳ thi kết thúc học phần đề thi và đáp án đề thi kết thúc học phần thực hiện theo hướng dẫn và quy định hiện hành của trường ĐHCT. 2. học phần thực hành điểm học phần được tính bằng điểm trung bình của các bài thực hành. 3. đối với các học phần có khối lượng nhỏ hơn 02 TC có thể chỉ có điểm của một loại hình đánh giá. 4. hình thức đánh giá trực tuyến được áp dụng khi đảm bảo trung thực, công bằng và khách quan như đánh giá trực tiếp, đồng thời đóng góp không quá 50% trọng số tổng điểm học phần riêng việc tổ chức bảo vệ và đánh giá luận văn tốt nghiệp được thực hiện trực tuyến với trọng số cao hơn khi đáp ứng thêm các điều kiện sau đây a việc đánh giá được thực hiện thông qua một hội đồng chuyên môn gồm ít nhất 3 thành viên b hình thức bảo vệ và đánh giá trực tuyến được sự đồng thuận của các thành viên hội đồng và người học c diễn biến của buổi bảo vệ trực tuyến được ghi hình, ghi âm đầy đủ và lưu trữ d việc tổ chức đánh giá luận văn tốt nghiệp theo hình thức trực tuyến được thực hiện như văn bản hướng dẫn hiện hành của hiệu trưởng về việc đánh giá luận văn tốt nghiệp theo hình thức trực tuyến. phương pháp đánh giá, hình thức đánh giá học phần, trọng số các điểm thành phần do GV đề xuất, trưởng bộ môn thuộc khoa, viện hoặc trung tâm hoặc trưởng khoa thuộc trường chuyên ngành, trưởng đơn vị đào tạo quản lý học phần duyệt và công bố trong đề cương chi tiết học phần tại trang thông tin điện tử của trường. </t>
   </si>
   <si>
-    <t xml:space="preserve">điều 22. điểm học phần 1. điểm đánh giá thành phần và điểm thi kết thúc học phần được chấm theo thang điểm 10 từ 0 đến 10, làm tròn đến một chữ số thập phân. 2. điểm học phần là tổng số điểm của tất cả các điểm đánh giá thành phần của học phần nhân với trọng số tương ứng. điểm học phần được tính theo thang điểm 10 và làm tròn đến một chữ số thập phân. GV phụ trách học phần nhập điểm vào hệ thống quản lý trực tuyến, hệ thống quy đổi sang điểm chữ và điểm số theo thang điểm 4. cách quy đổi điểm được thực hiện theo bảng dưới đây  điểm số theo thang điểm 10  điểm chữ  điểm số theo thang điểm 4  -----------------------------------------------------------------  9.0 - 10.0  A  4.0   8.0 - 8.9  B+  3.3   7.0 - 7.9  B  3.0   6.5 - 6.9  C+  2.5   5.5 - 6.4  C  2.0   5.0 - 5.4  D+  1.5   4.0 - 4.9  D  1.0   nhỏ hơn 4.0  F  0.0  3. học phần chỉ được tính tích lũy khi đạt từ điểm D trở lên. 4. điểm học phần sẽ được công bố và ghi nhận với điểm số theo thang điểm 10 và điểm chữ. điểm chữ được quy đổi sang điểm số theo thang điểm 4 để tính ĐTBCHK và ĐTBCTL xem điều 24. 5. các điểm học phần khác a điểm M tương đương điểm R của thông tư 08/2021/TT-BGDĐT dùng để xác nhận học phần SV được miễn học do đã tích lũy được bằng các hình thức khác. điểm M không được tính vào ĐTBCHK và ĐTBCTL. số TC của học phần có điểm M được tính vào tổng số TC tích lũy. để nhận điểm M, SV phải làm đơn có ý kiến của trưởng đơn vị đào tạo xem xét theo từng HK, kèm theo giấy tờ hợp lệ. b điểm I chỉ áp dụng cho đánh giá kết thúc học phần. dành cho các trường hợp SV đã dự học, dự các lần kiểm tra giữa HK, đã thực hiện các hoạt động liên quan đến học phần như thí nghiệm, thực hành nhưng vì lý do bất khả kháng như ốm đau, tai nạn,... đã vắng mặt trong buổi thi kết thúc học phần và được GV phụ trách học phần chấp thuận cho bổ sung điểm. điểm I không được tính vào ĐTBCHK ở HK đó. để nhận được điểm I, SV phải làm đơn kèm theo hồ sơ hợp lệ nộp cho GV giảng dạy học phần xem xét và trình trưởng đơn vị đào tạo duyệt. thời hạn bổ sung điểm của học phần do GV quy định nhưng không quá 1 năm kể từ ngày thi lần trước. qua thời hạn trên, nếu SV không hoàn thành thì học phần sẽ nhận điểm F. c điểm W dành cho các học phần mà SV được phép rút theo quy định xem điều 15. điểm W không tính vào ĐTBCHK và ĐTBCTL. </t>
-  </si>
-  <si>
     <t>điều 23. số lần thi, tổ chức thi và vắng thi 1. kỳ thi kết thúc học phần được tổ chức 1 lần. 2. thời gian tổ chức thi được thực hiện theo quy định xem điều 6. đối với các học phần riêng lẻ, GV tự sắp xếp để tổ chức thi thông qua hệ thống quản lý trực tuyến của trường ĐHCT đối với các học phần có nhiều SV, được giảng dạy nhiều lớp học phần thì có thể thi theo hình chung do đơn vị quản lý học phần quyết định và xếp lịch thi. lịch thi kết thúc học phần được công bố trên hệ thống quản lý trực tuyến và được GV thông báo đến tất cả SV chậm nhất 1 tuần trước ngày thi. 3. trong thời gian thi kết thúc học phần, nếu SV có lý do chính đáng không thể dự thi, được CVHT và GV giảng dạy học phần chấp thuận thì được phép vắng thi. sinh viên được phép vắng thi sẽ nhận điểm I theo quy định xem điểm b khoản 5 điều 22. điều 24. điểm trung bình chung học kỳ, điểm trung bình chung năm học và điểm trung bình chung tích lũy 1. số TC tích lũy là tổng số TC của các học phần đã tích lũy. 2. điểm trung bình chung học kỳ là trung bình có trọng số của điểm các học phần mà SV đã học trong HK kể cả các học phần bị điểm F và học phần điều kiện trừ học phần GDTC, với trọng số là số TC của các học phần đó. ĐTBCHK là cơ sở để đánh giá kết quả học tập, xét học bổng, khen thưởng, cảnh báo học tập sau mỗi HK. ĐTBCHK được tính theo công thức như sau \ \textđtbchk  \frac\sum_i1n x_i \cdot a_i\sum_i1n a_i \ trong đó - \x_i\ là điểm học phần thứ \i\ - \a_i\ là số TC của học phần thứ \i\ - \n\ là số học phần SV đăng ký học trong HK. 3. điểm trung bình chung năm học là trung bình có trọng số của điểm các học phần mà SV đã học trong năm học kể cả các học phần bị điểm F và học phần điều kiện trừ học phần GDTC. 4. điểm trung bình chung tích lũy là trung bình có trọng số của điểm các học phần đã tích lũy tính đến thời điểm xét không bao gồm các học phần bị điểm F và học phần điều kiện. ĐTBCTL là cơ sở để đánh giá kết quả học tập trong suốt thời gian học, xếp loại học tập, xếp hạng tốt nghiệp. 5. xếp loại học tập HK căn cứ vào ĐTBCHK xếp loại học tập năm học căn cứ vào ĐTBCNH theo bảng sau  xếp loại  ĐTBCHK/ĐTBCNH  ---------------------------  xuất sắc  3.60 - 4.00   giỏi  3.20 - 3.59   khá  2.50 - 3.19   trung bình  2.00 - 2.49   yếu  1.00 - 1.99   kém   1.00   điều 25. điểm rèn luyện 1. mức độ rèn luyện của SV được đánh giá từng HK và đo lường bằng ĐRL được chấm theo thang điểm 100 dựa vào các quy định hiện hành. ĐRL cả năm là trung bình cộng của ĐRL 3 HK. 2. sinh viên bị kỷ luật mức khiển trách cấp trường, khi đánh giá kết quả rèn luyện không được vượt quá loại khá. 3. sinh viên bị kỷ luật mức cảnh cáo cấp trường, khi đánh giá kết quả rèn luyện không được vượt quá loại trung bình. 4. sinh viên không thực hiện bảng đánh giá kết quả rèn luyện hoặc không nộp bảng đánh giá đúng thời gian quy định sẽ bị xếp loại kém ở HK đó. 5. sinh viên bị xếp loại rèn luyện yếu, kém trong 2 HK liên tiếp sẽ bị đình chỉ học tập 1 HK. 6. sinh viên bị xếp loại rèn luyện yếu, kém trong 2 HK liên tiếp lần thứ hai sẽ bị buộc thôi học. 7. sử dụng điểm rèn luyện a điểm rèn luyện toàn khóa học được lưu trong hồ sơ quản lý SV, ghi vào phụ lục văn bằng tốt nghiệp của SV. b điểm rèn luyện của SV từng HK là tiêu chí để xét HBKKHT, xếp loại và khen thưởng cuối mỗi năm học.</t>
   </si>
   <si>
@@ -125,6 +122,9 @@
   </si>
   <si>
     <t xml:space="preserve">điều 33. xử lý sinh viên quá hạn thời gian học tập 1. khi hết thời gian học tập tối đa theo quy định xem điều 5, những SV không đủ điều kiện tốt nghiệp sẽ bị xóa tên. 2. sinh viên đã hết thời gian học tập tối đa theo quy định nhưng chưa đủ điều kiện tốt nghiệp do chưa hoàn thành những học phần GDQPAN hoặc GDTC, trong thời hạn 5 năm tính từ khi thôi học SV được phép trở về trường ĐHCT để hoàn thiện các điều kiện còn thiếu và đề nghị xét công nhận tốt nghiệp. đối với SV từ khóa 47 trở về sau, SV đã hết thời gian học tập tối đa theo quy định nhưng chưa đủ điều kiện tốt nghiệp do chưa hoàn thành những học phần GDQPAN hoặc GDTC hoặc chưa đạt chuẩn đầu ra về ngoại ngữ, công nghệ thông tin, trong thời hạn 3 năm tính từ khi thôi học SV được phép trở về trường ĐHCT để hoàn thiện các điều kiện còn thiếu và đề nghị xét công nhận tốt nghiệp. 3. sinh viên không đủ điều kiện tốt nghiệp sẽ được trường bảo lưu, công nhận kết quả học tập đã tích lũy và cấp bảng điểm các học phần đã tích lũy nếu có yêu cầu. 4. sinh viên hết thời gian học hình thức chính quy được chuyển qua học hình thức vừa làm vừa học, hình thức đào tạo từ xa tương ứng nếu có của trường ĐHCT nếu còn trong thời gian học tập theo quy định đối với hình thức đào tạo chuyển đến. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">điều 22. điểm học phần 1. điểm đánh giá thành phần và điểm thi kết thúc học phần được chấm theo thang điểm 10 từ 0 đến 10, làm tròn đến một chữ số thập phân. 2. điểm học phần là tổng số điểm của tất cả các điểm đánh giá thành phần của học phần nhân với trọng số tương ứng. điểm học phần được tính theo thang điểm 10 và làm tròn đến một chữ số thập phân. GV phụ trách học phần nhập điểm vào hệ thống quản lý trực tuyến, hệ thống quy đổi sang điểm chữ và điểm số theo thang điểm 4. cách quy đổi điểm được thực hiện theo bảng dưới đây  điểm số theo thang điểm 10  điểm chữ  điểm số theo thang điểm 4  -----------------------------------------------------------------  9.0 - 10.0  A  4.0   8.0 - 8.9  B+  3.5   7.0 - 7.9  B  3.0   6.5 - 6.9  C+  2.5   5.5 - 6.4  C  2.0   5.0 - 5.4  D+  1.5   4.0 - 4.9  D  1.0   nhỏ hơn 4.0  F  0.0  3. học phần chỉ được tính tích lũy khi đạt từ điểm D trở lên. 4. điểm học phần sẽ được công bố và ghi nhận với điểm số theo thang điểm 10 và điểm chữ. điểm chữ được quy đổi sang điểm số theo thang điểm 4 để tính ĐTBCHK và ĐTBCTL xem điều 24. 5. các điểm học phần khác a điểm M tương đương điểm R của thông tư 08/2021/TT-BGDĐT dùng để xác nhận học phần SV được miễn học do đã tích lũy được bằng các hình thức khác. điểm M không được tính vào ĐTBCHK và ĐTBCTL. số TC của học phần có điểm M được tính vào tổng số TC tích lũy. để nhận điểm M, SV phải làm đơn có ý kiến của trưởng đơn vị đào tạo xem xét theo từng HK, kèm theo giấy tờ hợp lệ. b điểm I chỉ áp dụng cho đánh giá kết thúc học phần. dành cho các trường hợp SV đã dự học, dự các lần kiểm tra giữa HK, đã thực hiện các hoạt động liên quan đến học phần như thí nghiệm, thực hành nhưng vì lý do bất khả kháng như ốm đau, tai nạn,... đã vắng mặt trong buổi thi kết thúc học phần và được GV phụ trách học phần chấp thuận cho bổ sung điểm. điểm I không được tính vào ĐTBCHK ở HK đó. để nhận được điểm I, SV phải làm đơn kèm theo hồ sơ hợp lệ nộp cho GV giảng dạy học phần xem xét và trình trưởng đơn vị đào tạo duyệt. thời hạn bổ sung điểm của học phần do GV quy định nhưng không quá 1 năm kể từ ngày thi lần trước. qua thời hạn trên, nếu SV không hoàn thành thì học phần sẽ nhận điểm F. c điểm W dành cho các học phần mà SV được phép rút theo quy định xem điều 15. điểm W không tính vào ĐTBCHK và ĐTBCTL. </t>
   </si>
 </sst>
 </file>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="99.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -647,7 +647,7 @@
     </row>
     <row r="19" spans="1:2" ht="232" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>19</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="20" spans="1:2" ht="319" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>19</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="21" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>9</v>
@@ -671,23 +671,23 @@
     </row>
     <row r="22" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>19</v>
@@ -695,7 +695,7 @@
     </row>
     <row r="25" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>19</v>
@@ -703,34 +703,34 @@
     </row>
     <row r="26" spans="1:2" ht="145" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -738,7 +738,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>